<commit_message>
update end of 2025
for Dr Meek at UoU
</commit_message>
<xml_diff>
--- a/data/admin.xlsx
+++ b/data/admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00315273\Documents\GitHub\jy_CV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00315273\GitHub\myCV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1511BF-4708-458D-948A-BE3CF957C035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E8FA91-C63B-45F7-A37A-68ADD5471677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{59DDEC0E-4715-4771-BF5C-FC5C9CC2B2D9}"/>
+    <workbookView xWindow="1245" yWindow="1950" windowWidth="27555" windowHeight="14130" xr2:uid="{59DDEC0E-4715-4771-BF5C-FC5C9CC2B2D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>order</t>
   </si>
@@ -82,19 +82,40 @@
   </si>
   <si>
     <t>Update pre-test question bank</t>
+  </si>
+  <si>
+    <t>2025-present</t>
+  </si>
+  <si>
+    <t>SONA Coordinator</t>
+  </si>
+  <si>
+    <t>Administer the participant recruitment system</t>
+  </si>
+  <si>
+    <t>Interface with USU researchers and the IRB</t>
+  </si>
+  <si>
+    <t>Troubleshoot with USU students and instructors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,9 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -138,9 +160,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +200,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -284,7 +306,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,7 +448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,19 +456,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BACE165-6410-430B-B7AC-4C8589D81A8E}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.1328125" customWidth="1"/>
-    <col min="3" max="3" width="10.9296875" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -486,30 +508,63 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="K16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>